<commit_message>
Delete the tests subtasks.
</commit_message>
<xml_diff>
--- a/Operatore/Tasks/Values and situations plus Parameters.xlsx
+++ b/Operatore/Tasks/Values and situations plus Parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11595" firstSheet="19" activeTab="23"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="initial settings" sheetId="16" r:id="rId1"/>
@@ -29,8 +29,6 @@
     <sheet name="sequence(Shutdown)" sheetId="35" r:id="rId20"/>
     <sheet name="sequence(Optical water level)" sheetId="37" r:id="rId21"/>
     <sheet name="sequence(Pressure control)" sheetId="38" r:id="rId22"/>
-    <sheet name="sequence(switch button)" sheetId="40" r:id="rId23"/>
-    <sheet name="sequence(switch button display)" sheetId="41" r:id="rId24"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -639,76 +637,6 @@
 </comments>
 </file>
 
-<file path=xl/comments23.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Autore</author>
-  </authors>
-  <commentList>
-    <comment ref="C6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autore:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-it is up to us to decide to use the same values as UNIGE (0,25) or integers
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments24.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Autore</author>
-  </authors>
-  <commentList>
-    <comment ref="C6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Autore:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-it is up to us to decide to use the same values as UNIGE (0,25) or integers
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
@@ -1102,7 +1030,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12774" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11701" uniqueCount="109">
   <si>
     <t>number</t>
   </si>
@@ -1429,24 +1357,6 @@
   </si>
   <si>
     <t>Livello acqua vaschetta</t>
-  </si>
-  <si>
-    <t>test of switches and button</t>
-  </si>
-  <si>
-    <t>switch button test</t>
-  </si>
-  <si>
-    <t>switch button action test</t>
-  </si>
-  <si>
-    <t>test of switches, button, and display</t>
-  </si>
-  <si>
-    <t>switch button display test</t>
-  </si>
-  <si>
-    <t>switch button display action test</t>
   </si>
 </sst>
 </file>
@@ -2269,10 +2179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE22"/>
+  <dimension ref="A1:AE20"/>
   <sheetViews>
-    <sheetView topLeftCell="E13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4179,196 +4089,6 @@
         <v>0</v>
       </c>
       <c r="AE20" s="42">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" ht="30">
-      <c r="A21" s="66">
-        <v>21</v>
-      </c>
-      <c r="B21" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" s="68" t="s">
-        <v>110</v>
-      </c>
-      <c r="D21" s="68" t="s">
-        <v>111</v>
-      </c>
-      <c r="E21" s="13">
-        <v>2</v>
-      </c>
-      <c r="F21" s="13">
-        <v>1</v>
-      </c>
-      <c r="G21" s="13">
-        <v>1</v>
-      </c>
-      <c r="H21" s="13">
-        <v>1</v>
-      </c>
-      <c r="I21" s="13">
-        <v>1</v>
-      </c>
-      <c r="J21" s="13">
-        <v>2</v>
-      </c>
-      <c r="K21" s="13">
-        <v>0</v>
-      </c>
-      <c r="L21" s="13">
-        <v>0</v>
-      </c>
-      <c r="M21" s="13">
-        <v>0</v>
-      </c>
-      <c r="N21" s="13">
-        <v>0</v>
-      </c>
-      <c r="O21" s="13">
-        <v>0</v>
-      </c>
-      <c r="P21" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="13">
-        <v>1</v>
-      </c>
-      <c r="R21" s="13">
-        <v>1</v>
-      </c>
-      <c r="S21" s="13">
-        <v>0</v>
-      </c>
-      <c r="T21" s="13">
-        <v>0</v>
-      </c>
-      <c r="U21" s="13">
-        <v>0</v>
-      </c>
-      <c r="V21" s="13">
-        <v>0</v>
-      </c>
-      <c r="W21" s="66">
-        <v>9</v>
-      </c>
-      <c r="X21" s="66">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="66">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="66">
-        <v>0</v>
-      </c>
-      <c r="AA21" s="66">
-        <v>0</v>
-      </c>
-      <c r="AB21" s="42">
-        <v>900000</v>
-      </c>
-      <c r="AC21" s="66">
-        <v>900</v>
-      </c>
-      <c r="AD21" s="66">
-        <v>0</v>
-      </c>
-      <c r="AE21" s="42">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" ht="45">
-      <c r="A22" s="66">
-        <v>22</v>
-      </c>
-      <c r="B22" s="67" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="68" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="68" t="s">
-        <v>114</v>
-      </c>
-      <c r="E22" s="13">
-        <v>2</v>
-      </c>
-      <c r="F22" s="13">
-        <v>1</v>
-      </c>
-      <c r="G22" s="13">
-        <v>1</v>
-      </c>
-      <c r="H22" s="13">
-        <v>1</v>
-      </c>
-      <c r="I22" s="13">
-        <v>1</v>
-      </c>
-      <c r="J22" s="13">
-        <v>2</v>
-      </c>
-      <c r="K22" s="13">
-        <v>0</v>
-      </c>
-      <c r="L22" s="13">
-        <v>0</v>
-      </c>
-      <c r="M22" s="13">
-        <v>0</v>
-      </c>
-      <c r="N22" s="13">
-        <v>0</v>
-      </c>
-      <c r="O22" s="13">
-        <v>0</v>
-      </c>
-      <c r="P22" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="13">
-        <v>1</v>
-      </c>
-      <c r="R22" s="13">
-        <v>1</v>
-      </c>
-      <c r="S22" s="13">
-        <v>0</v>
-      </c>
-      <c r="T22" s="13">
-        <v>0</v>
-      </c>
-      <c r="U22" s="13">
-        <v>0</v>
-      </c>
-      <c r="V22" s="13">
-        <v>0</v>
-      </c>
-      <c r="W22" s="66">
-        <v>5</v>
-      </c>
-      <c r="X22" s="66">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="66">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="66">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="66">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="42">
-        <v>900000</v>
-      </c>
-      <c r="AC22" s="66">
-        <v>900</v>
-      </c>
-      <c r="AD22" s="66">
-        <v>0</v>
-      </c>
-      <c r="AE22" s="42">
         <v>10</v>
       </c>
     </row>
@@ -26801,10 +26521,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView topLeftCell="H16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A22" sqref="A21:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -28198,142 +27918,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:22" customFormat="1" ht="30">
-      <c r="A21" s="66">
-        <v>21</v>
-      </c>
-      <c r="B21" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" s="68" t="s">
-        <v>110</v>
-      </c>
-      <c r="D21" s="68" t="s">
-        <v>111</v>
-      </c>
-      <c r="E21" s="13">
-        <v>0</v>
-      </c>
-      <c r="F21" s="13">
-        <v>0</v>
-      </c>
-      <c r="G21" s="13">
-        <v>0</v>
-      </c>
-      <c r="H21" s="13">
-        <v>0</v>
-      </c>
-      <c r="I21" s="13">
-        <v>0</v>
-      </c>
-      <c r="J21" s="13">
-        <v>0</v>
-      </c>
-      <c r="K21" s="13">
-        <v>0</v>
-      </c>
-      <c r="L21" s="13">
-        <v>1</v>
-      </c>
-      <c r="M21" s="13">
-        <v>0</v>
-      </c>
-      <c r="N21" s="13">
-        <v>0</v>
-      </c>
-      <c r="O21" s="13">
-        <v>0</v>
-      </c>
-      <c r="P21" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="13">
-        <v>1</v>
-      </c>
-      <c r="R21" s="13">
-        <v>1</v>
-      </c>
-      <c r="S21" s="13">
-        <v>0</v>
-      </c>
-      <c r="T21" s="13">
-        <v>0</v>
-      </c>
-      <c r="U21" s="13">
-        <v>0</v>
-      </c>
-      <c r="V21" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" customFormat="1" ht="30">
-      <c r="A22" s="66">
-        <v>22</v>
-      </c>
-      <c r="B22" s="67" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="68" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="68" t="s">
-        <v>114</v>
-      </c>
-      <c r="E22" s="13">
-        <v>0</v>
-      </c>
-      <c r="F22" s="13">
-        <v>0</v>
-      </c>
-      <c r="G22" s="13">
-        <v>0</v>
-      </c>
-      <c r="H22" s="13">
-        <v>0</v>
-      </c>
-      <c r="I22" s="13">
-        <v>0</v>
-      </c>
-      <c r="J22" s="13">
-        <v>0</v>
-      </c>
-      <c r="K22" s="13">
-        <v>0</v>
-      </c>
-      <c r="L22" s="13">
-        <v>1</v>
-      </c>
-      <c r="M22" s="13">
-        <v>0</v>
-      </c>
-      <c r="N22" s="13">
-        <v>0</v>
-      </c>
-      <c r="O22" s="13">
-        <v>0</v>
-      </c>
-      <c r="P22" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="13">
-        <v>1</v>
-      </c>
-      <c r="R22" s="13">
-        <v>1</v>
-      </c>
-      <c r="S22" s="13">
-        <v>0</v>
-      </c>
-      <c r="T22" s="13">
-        <v>0</v>
-      </c>
-      <c r="U22" s="13">
-        <v>0</v>
-      </c>
-      <c r="V22" s="13">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -30387,7 +29971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U64"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="P68" sqref="P68"/>
     </sheetView>
   </sheetViews>
@@ -34437,7 +34021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U64"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection sqref="A1:U32"/>
     </sheetView>
   </sheetViews>
@@ -38485,4092 +38069,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U32"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:21" ht="45">
-      <c r="A1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="65" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" s="4">
-        <v>8</v>
-      </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="69" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="9">
-        <v>8</v>
-      </c>
-      <c r="L2" s="9">
-        <v>12</v>
-      </c>
-      <c r="M2" s="9">
-        <v>13</v>
-      </c>
-      <c r="N2" s="9">
-        <v>17</v>
-      </c>
-      <c r="O2" s="9">
-        <v>19</v>
-      </c>
-      <c r="P2" s="9">
-        <v>21.1</v>
-      </c>
-      <c r="Q2" s="9">
-        <v>21.2</v>
-      </c>
-      <c r="R2" s="10">
-        <v>22</v>
-      </c>
-      <c r="S2" s="10">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="105">
-      <c r="A3" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="O3" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="P3" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="S3" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="T3" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="U3" s="19" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="30">
-      <c r="A4" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="64">
-        <v>1</v>
-      </c>
-      <c r="C4" s="64">
-        <v>2</v>
-      </c>
-      <c r="D4" s="64">
-        <v>2</v>
-      </c>
-      <c r="E4" s="64">
-        <v>2</v>
-      </c>
-      <c r="F4" s="64">
-        <v>2</v>
-      </c>
-      <c r="G4" s="64">
-        <v>3</v>
-      </c>
-      <c r="H4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="64">
-        <v>4</v>
-      </c>
-      <c r="J4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="O4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="P4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="R4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="S4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="T4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="U4" s="64" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="26">
-        <v>0</v>
-      </c>
-      <c r="C5" s="16">
-        <v>0</v>
-      </c>
-      <c r="D5" s="16">
-        <v>0</v>
-      </c>
-      <c r="E5" s="16">
-        <v>0</v>
-      </c>
-      <c r="F5" s="16">
-        <v>0</v>
-      </c>
-      <c r="G5" s="16">
-        <v>0</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T5" s="16">
-        <v>2</v>
-      </c>
-      <c r="U5" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="26">
-        <v>0</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="16">
-        <v>0</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T6" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="U6" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="A7" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="26">
-        <v>0</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="16">
-        <v>0</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T7" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="U7" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
-      <c r="A8" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="26">
-        <v>0</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="16">
-        <v>0</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T8" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="U8" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="A9" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="26">
-        <v>0</v>
-      </c>
-      <c r="G9" s="16">
-        <v>0</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T9" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="U9" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
-      <c r="A10" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="26">
-        <v>0</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T10" s="16">
-        <v>2</v>
-      </c>
-      <c r="U10" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
-      <c r="A11" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="26">
-        <v>0</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T11" s="16">
-        <v>1</v>
-      </c>
-      <c r="U11" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
-      <c r="A12" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="26">
-        <v>1</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T12" s="16">
-        <v>0</v>
-      </c>
-      <c r="U12" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
-      <c r="A13" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="26">
-        <v>0</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T13" s="16">
-        <v>0</v>
-      </c>
-      <c r="U13" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
-      <c r="A14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="16">
-        <v>1</v>
-      </c>
-      <c r="K14" s="26">
-        <v>1</v>
-      </c>
-      <c r="L14" s="16">
-        <v>1</v>
-      </c>
-      <c r="M14" s="16">
-        <v>1</v>
-      </c>
-      <c r="N14" s="16">
-        <v>1</v>
-      </c>
-      <c r="O14" s="16">
-        <v>1</v>
-      </c>
-      <c r="P14" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="16">
-        <v>1</v>
-      </c>
-      <c r="R14" s="16">
-        <v>1</v>
-      </c>
-      <c r="S14" s="16">
-        <v>1</v>
-      </c>
-      <c r="T14" s="16">
-        <v>1</v>
-      </c>
-      <c r="U14" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21">
-      <c r="A15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J15" s="16">
-        <v>1</v>
-      </c>
-      <c r="K15" s="16">
-        <v>1</v>
-      </c>
-      <c r="L15" s="26">
-        <v>1</v>
-      </c>
-      <c r="M15" s="16">
-        <v>1</v>
-      </c>
-      <c r="N15" s="16">
-        <v>1</v>
-      </c>
-      <c r="O15" s="16">
-        <v>1</v>
-      </c>
-      <c r="P15" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="16">
-        <v>1</v>
-      </c>
-      <c r="R15" s="16">
-        <v>1</v>
-      </c>
-      <c r="S15" s="16">
-        <v>1</v>
-      </c>
-      <c r="T15" s="16">
-        <v>1</v>
-      </c>
-      <c r="U15" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21">
-      <c r="A16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="16">
-        <v>0</v>
-      </c>
-      <c r="K16" s="16">
-        <v>0</v>
-      </c>
-      <c r="L16" s="16">
-        <v>0</v>
-      </c>
-      <c r="M16" s="26">
-        <v>0</v>
-      </c>
-      <c r="N16" s="16">
-        <v>0</v>
-      </c>
-      <c r="O16" s="16">
-        <v>0</v>
-      </c>
-      <c r="P16" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="16">
-        <v>0</v>
-      </c>
-      <c r="R16" s="16">
-        <v>0</v>
-      </c>
-      <c r="S16" s="16">
-        <v>0</v>
-      </c>
-      <c r="T16" s="16">
-        <v>0</v>
-      </c>
-      <c r="U16" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21">
-      <c r="A17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" s="16">
-        <v>1</v>
-      </c>
-      <c r="K17" s="16">
-        <v>1</v>
-      </c>
-      <c r="L17" s="16">
-        <v>1</v>
-      </c>
-      <c r="M17" s="16">
-        <v>1</v>
-      </c>
-      <c r="N17" s="26">
-        <v>1</v>
-      </c>
-      <c r="O17" s="16">
-        <v>1</v>
-      </c>
-      <c r="P17" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="16">
-        <v>1</v>
-      </c>
-      <c r="R17" s="16">
-        <v>1</v>
-      </c>
-      <c r="S17" s="16">
-        <v>1</v>
-      </c>
-      <c r="T17" s="16">
-        <v>1</v>
-      </c>
-      <c r="U17" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21">
-      <c r="A18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" s="16">
-        <v>0</v>
-      </c>
-      <c r="K18" s="16">
-        <v>0</v>
-      </c>
-      <c r="L18" s="16">
-        <v>0</v>
-      </c>
-      <c r="M18" s="16">
-        <v>0</v>
-      </c>
-      <c r="N18" s="16">
-        <v>0</v>
-      </c>
-      <c r="O18" s="26">
-        <v>0</v>
-      </c>
-      <c r="P18" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="16">
-        <v>0</v>
-      </c>
-      <c r="R18" s="16">
-        <v>0</v>
-      </c>
-      <c r="S18" s="16">
-        <v>0</v>
-      </c>
-      <c r="T18" s="16">
-        <v>0</v>
-      </c>
-      <c r="U18" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
-      <c r="A19" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P19" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R19" s="16">
-        <v>1</v>
-      </c>
-      <c r="S19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T19" s="16">
-        <v>1</v>
-      </c>
-      <c r="U19" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
-      <c r="A20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q20" s="26">
-        <v>1</v>
-      </c>
-      <c r="R20" s="16">
-        <v>1</v>
-      </c>
-      <c r="S20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T20" s="16">
-        <v>1</v>
-      </c>
-      <c r="U20" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
-      <c r="A21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K21" s="16">
-        <v>0</v>
-      </c>
-      <c r="L21" s="16">
-        <v>0</v>
-      </c>
-      <c r="M21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R21" s="63">
-        <v>0</v>
-      </c>
-      <c r="S21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T21" s="16">
-        <v>0</v>
-      </c>
-      <c r="U21" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="90">
-      <c r="A22" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S22" s="63">
-        <v>0</v>
-      </c>
-      <c r="T22" s="16">
-        <v>1</v>
-      </c>
-      <c r="U22" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="60">
-      <c r="A23" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T23" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="U23" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="45">
-      <c r="A24" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="16">
-        <v>10</v>
-      </c>
-      <c r="J24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T24" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="U24" s="26" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
-      <c r="A25" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="U25" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21">
-      <c r="A26" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="J26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="K26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="L26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="M26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="N26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="O26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="P26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="R26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="S26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="T26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="U26" s="62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21">
-      <c r="A27" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="B27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="H27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="K27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="L27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="M27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="N27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="O27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="P27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="R27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="S27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="T27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="U27" s="62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21">
-      <c r="A28" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="K28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="L28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="M28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="N28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="O28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="P28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="R28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="S28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="T28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="U28" s="62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
-      <c r="A29" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="K29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="L29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="M29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="N29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="O29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="P29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="R29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="S29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="T29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="U29" s="62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21">
-      <c r="A30" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="B30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="K30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="L30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="M30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="N30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="O30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="P30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="R30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="S30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="T30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="U30" s="62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21">
-      <c r="A31" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="J31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="K31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="L31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="M31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="N31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="O31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="P31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="R31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="S31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="T31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="U31" s="62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21">
-      <c r="A32" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="B32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="K32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="L32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="M32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="N32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="O32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="P32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="R32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="S32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="T32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="U32" s="62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:J2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U32"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="43.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" ht="45">
-      <c r="A1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="65" t="s">
-        <v>114</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" s="4">
-        <v>8</v>
-      </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="69" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="9">
-        <v>8</v>
-      </c>
-      <c r="L2" s="9">
-        <v>12</v>
-      </c>
-      <c r="M2" s="9">
-        <v>13</v>
-      </c>
-      <c r="N2" s="9">
-        <v>17</v>
-      </c>
-      <c r="O2" s="9">
-        <v>19</v>
-      </c>
-      <c r="P2" s="9">
-        <v>21.1</v>
-      </c>
-      <c r="Q2" s="9">
-        <v>21.2</v>
-      </c>
-      <c r="R2" s="10">
-        <v>22</v>
-      </c>
-      <c r="S2" s="10">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="105">
-      <c r="A3" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="O3" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="P3" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="S3" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="T3" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="U3" s="19" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="30">
-      <c r="A4" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="64">
-        <v>1</v>
-      </c>
-      <c r="C4" s="64">
-        <v>2</v>
-      </c>
-      <c r="D4" s="64">
-        <v>2</v>
-      </c>
-      <c r="E4" s="64">
-        <v>2</v>
-      </c>
-      <c r="F4" s="64">
-        <v>2</v>
-      </c>
-      <c r="G4" s="64">
-        <v>3</v>
-      </c>
-      <c r="H4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="64">
-        <v>4</v>
-      </c>
-      <c r="J4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="O4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="P4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="R4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="S4" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="T4" s="64">
-        <v>5</v>
-      </c>
-      <c r="U4" s="64" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="26">
-        <v>0</v>
-      </c>
-      <c r="C5" s="16">
-        <v>0</v>
-      </c>
-      <c r="D5" s="16">
-        <v>0</v>
-      </c>
-      <c r="E5" s="16">
-        <v>0</v>
-      </c>
-      <c r="F5" s="16">
-        <v>0</v>
-      </c>
-      <c r="G5" s="16">
-        <v>0</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T5" s="16">
-        <v>0</v>
-      </c>
-      <c r="U5" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="26">
-        <v>0</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="16">
-        <v>0</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T6" s="16">
-        <v>0</v>
-      </c>
-      <c r="U6" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="A7" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="26">
-        <v>0</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="16">
-        <v>0</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T7" s="16">
-        <v>0</v>
-      </c>
-      <c r="U7" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
-      <c r="A8" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="26">
-        <v>0</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="16">
-        <v>0</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T8" s="16">
-        <v>0</v>
-      </c>
-      <c r="U8" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="A9" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="26">
-        <v>0</v>
-      </c>
-      <c r="G9" s="16">
-        <v>0</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T9" s="16">
-        <v>0</v>
-      </c>
-      <c r="U9" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
-      <c r="A10" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="26">
-        <v>0</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T10" s="16">
-        <v>0</v>
-      </c>
-      <c r="U10" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
-      <c r="A11" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="26">
-        <v>0</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="U11" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
-      <c r="A12" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="26">
-        <v>1</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T12" s="16">
-        <v>1</v>
-      </c>
-      <c r="U12" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
-      <c r="A13" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="26">
-        <v>0</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="U13" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
-      <c r="A14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="16">
-        <v>1</v>
-      </c>
-      <c r="K14" s="26">
-        <v>1</v>
-      </c>
-      <c r="L14" s="16">
-        <v>1</v>
-      </c>
-      <c r="M14" s="16">
-        <v>1</v>
-      </c>
-      <c r="N14" s="16">
-        <v>1</v>
-      </c>
-      <c r="O14" s="16">
-        <v>1</v>
-      </c>
-      <c r="P14" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="16">
-        <v>1</v>
-      </c>
-      <c r="R14" s="16">
-        <v>1</v>
-      </c>
-      <c r="S14" s="16">
-        <v>1</v>
-      </c>
-      <c r="T14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="U14" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21">
-      <c r="A15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J15" s="16">
-        <v>1</v>
-      </c>
-      <c r="K15" s="16">
-        <v>1</v>
-      </c>
-      <c r="L15" s="26">
-        <v>1</v>
-      </c>
-      <c r="M15" s="16">
-        <v>1</v>
-      </c>
-      <c r="N15" s="16">
-        <v>1</v>
-      </c>
-      <c r="O15" s="16">
-        <v>1</v>
-      </c>
-      <c r="P15" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="16">
-        <v>1</v>
-      </c>
-      <c r="R15" s="16">
-        <v>1</v>
-      </c>
-      <c r="S15" s="16">
-        <v>1</v>
-      </c>
-      <c r="T15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="U15" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21">
-      <c r="A16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="16">
-        <v>0</v>
-      </c>
-      <c r="K16" s="16">
-        <v>0</v>
-      </c>
-      <c r="L16" s="16">
-        <v>0</v>
-      </c>
-      <c r="M16" s="26">
-        <v>0</v>
-      </c>
-      <c r="N16" s="16">
-        <v>0</v>
-      </c>
-      <c r="O16" s="16">
-        <v>0</v>
-      </c>
-      <c r="P16" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="16">
-        <v>0</v>
-      </c>
-      <c r="R16" s="16">
-        <v>0</v>
-      </c>
-      <c r="S16" s="16">
-        <v>0</v>
-      </c>
-      <c r="T16" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="U16" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21">
-      <c r="A17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" s="16">
-        <v>1</v>
-      </c>
-      <c r="K17" s="16">
-        <v>1</v>
-      </c>
-      <c r="L17" s="16">
-        <v>1</v>
-      </c>
-      <c r="M17" s="16">
-        <v>1</v>
-      </c>
-      <c r="N17" s="26">
-        <v>1</v>
-      </c>
-      <c r="O17" s="16">
-        <v>1</v>
-      </c>
-      <c r="P17" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="16">
-        <v>1</v>
-      </c>
-      <c r="R17" s="16">
-        <v>1</v>
-      </c>
-      <c r="S17" s="16">
-        <v>1</v>
-      </c>
-      <c r="T17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="U17" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21">
-      <c r="A18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" s="16">
-        <v>0</v>
-      </c>
-      <c r="K18" s="16">
-        <v>0</v>
-      </c>
-      <c r="L18" s="16">
-        <v>0</v>
-      </c>
-      <c r="M18" s="16">
-        <v>0</v>
-      </c>
-      <c r="N18" s="16">
-        <v>0</v>
-      </c>
-      <c r="O18" s="26">
-        <v>0</v>
-      </c>
-      <c r="P18" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="16">
-        <v>0</v>
-      </c>
-      <c r="R18" s="16">
-        <v>0</v>
-      </c>
-      <c r="S18" s="16">
-        <v>0</v>
-      </c>
-      <c r="T18" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="U18" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
-      <c r="A19" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P19" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R19" s="16">
-        <v>1</v>
-      </c>
-      <c r="S19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="U19" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
-      <c r="A20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q20" s="26">
-        <v>1</v>
-      </c>
-      <c r="R20" s="16">
-        <v>1</v>
-      </c>
-      <c r="S20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="U20" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
-      <c r="A21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K21" s="16">
-        <v>0</v>
-      </c>
-      <c r="L21" s="16">
-        <v>0</v>
-      </c>
-      <c r="M21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R21" s="63">
-        <v>0</v>
-      </c>
-      <c r="S21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="U21" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="90">
-      <c r="A22" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S22" s="63">
-        <v>0</v>
-      </c>
-      <c r="T22" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="U22" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="60">
-      <c r="A23" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S23" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T23" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="U23" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="45">
-      <c r="A24" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T24" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="U24" s="26" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
-      <c r="A25" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="O25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="S25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="T25" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="U25" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21">
-      <c r="A26" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="B26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="J26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="K26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="L26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="M26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="N26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="O26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="P26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="R26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="S26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="T26" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="U26" s="62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21">
-      <c r="A27" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="B27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="H27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="K27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="L27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="M27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="N27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="O27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="P27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="R27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="S27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="T27" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="U27" s="62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21">
-      <c r="A28" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="K28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="L28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="M28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="N28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="O28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="P28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="R28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="S28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="T28" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="U28" s="62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
-      <c r="A29" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="K29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="L29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="M29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="N29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="O29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="P29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="R29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="S29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="T29" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="U29" s="62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21">
-      <c r="A30" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="B30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="K30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="L30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="M30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="N30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="O30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="P30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="R30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="S30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="T30" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="U30" s="62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21">
-      <c r="A31" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="J31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="K31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="L31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="M31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="N31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="O31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="P31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="R31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="S31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="T31" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="U31" s="62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21">
-      <c r="A32" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="B32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="K32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="L32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="M32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="N32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="O32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="P32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="R32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="S32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="T32" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="U32" s="62" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:J2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A22" sqref="A21:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42920,40 +38424,6 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30">
-      <c r="A21" s="66">
-        <v>21</v>
-      </c>
-      <c r="B21" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" s="68" t="s">
-        <v>110</v>
-      </c>
-      <c r="D21" s="68" t="s">
-        <v>111</v>
-      </c>
-      <c r="E21" s="44" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30">
-      <c r="A22" s="66">
-        <v>22</v>
-      </c>
-      <c r="B22" s="67" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="68" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="68" t="s">
-        <v>114</v>
-      </c>
-      <c r="E22" s="44" t="s">
-        <v>67</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -42965,8 +38435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>